<commit_message>
now the number works
</commit_message>
<xml_diff>
--- a/template/template-target.xlsx
+++ b/template/template-target.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liajiang/Developers/BOL/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA7DA71-C1BE-7644-87D1-F5942F8B6440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AB9CF-75E0-714E-B2C4-DB0CA49BB1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,56 +246,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Fee Terms:    Collect:  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <charset val="2"/>
-      </rPr>
-      <t>¨</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    Prepaid: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <charset val="2"/>
-      </rPr>
-      <t>o</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Customer check acceptable: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <charset val="2"/>
-      </rPr>
-      <t>o</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">NOTE  Liability Limitation for loss or damage in this shipment may be applicable.  See 49 U.S.C. </t>
     </r>
     <r>
@@ -468,12 +418,18 @@
   <si>
     <t>☐  By Driver/Pieces</t>
   </si>
+  <si>
+    <t>Fee Terms:    Collect:  ☐    Prepaid: ☐</t>
+  </si>
+  <si>
+    <t>Customer check acceptable: ☐</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,13 +584,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9.5"/>
-      <color theme="1"/>
-      <name val="Wingdings"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="8.5"/>
       <color theme="1"/>
       <name val="Mono821CECP BT"/>
@@ -1014,7 +963,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1071,17 +1020,337 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,27 +1406,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1186,305 +1434,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1947,7 +1896,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A33" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="I44" sqref="I44:M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1960,448 +1909,448 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="140"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="64"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="161"/>
+      <c r="M1" s="162"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="129"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="32" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="133"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="32" t="s">
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="139"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="77" t="s">
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="79"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="91"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="79"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="91"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="82"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="94"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="67"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="163" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="164"/>
+      <c r="J8" s="164"/>
+      <c r="K8" s="164"/>
+      <c r="L8" s="164"/>
+      <c r="M8" s="165"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="55" t="s">
+      <c r="A9" s="146" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="147"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="57"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="79"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="53" t="s">
+      <c r="A10" s="160" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="113"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="82"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="114" t="s">
-        <v>89</v>
-      </c>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="115"/>
-      <c r="M11" s="116"/>
+      <c r="A11" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="85"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
       <c r="G12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="117" t="s">
+      <c r="H12" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="118"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="118"/>
-      <c r="M12" s="119"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="88"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="77" t="s">
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="79"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="91"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="79"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="91"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="82"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="94"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="114" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="115"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="116"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="85"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
-      <c r="K17" s="121"/>
-      <c r="L17" s="121"/>
-      <c r="M17" s="122"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="97"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="86" t="s">
+      <c r="B18" s="136"/>
+      <c r="C18" s="136"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87" t="s">
+      <c r="I18" s="63"/>
+      <c r="J18" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87" t="s">
+      <c r="K18" s="63"/>
+      <c r="L18" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="88"/>
+      <c r="M18" s="64"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="129" t="s">
+      <c r="A19" s="77"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="130"/>
-      <c r="J19" s="125" t="s">
+      <c r="I19" s="108"/>
+      <c r="J19" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="126"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="104"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="58" t="s">
+      <c r="A20" s="80"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="156" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="59"/>
-      <c r="J20" s="127"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="128"/>
+      <c r="I20" s="157"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="106"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
+      <c r="H21" s="159"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="159"/>
+      <c r="K21" s="159"/>
+      <c r="L21" s="159"/>
+      <c r="M21" s="159"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="47" t="s">
+      <c r="H22" s="152" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="48"/>
-      <c r="J22" s="83" t="s">
+      <c r="I22" s="153"/>
+      <c r="J22" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="85"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="92"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="49" t="s">
+      <c r="A23" s="138"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="50"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="88"/>
+      <c r="I23" s="155"/>
+      <c r="J23" s="134"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="64"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="12" t="str">
         <f>IF(B24="", "", "PO#")</f>
         <v/>
       </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="124"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="102"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="9" t="s">
@@ -2410,20 +2359,20 @@
       <c r="I24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="12" t="str">
         <f t="shared" ref="A25:A26" si="0">IF(B25="", "", "PO#")</f>
         <v/>
       </c>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="124"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="102"/>
       <c r="F25" s="17"/>
       <c r="G25" s="19"/>
       <c r="H25" s="6" t="s">
@@ -2432,20 +2381,20 @@
       <c r="I25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="124"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="102"/>
       <c r="F26" s="17"/>
       <c r="G26" s="19"/>
       <c r="H26" s="6" t="s">
@@ -2454,19 +2403,19 @@
       <c r="I26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="13">
         <f>F24+F25</f>
         <v>0</v>
@@ -2475,102 +2424,102 @@
         <f>G24+G25</f>
         <v>0</v>
       </c>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="94"/>
-      <c r="L27" s="94"/>
-      <c r="M27" s="94"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="95"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="111"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="137" t="s">
+      <c r="A29" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="137"/>
-      <c r="C29" s="51" t="s">
+      <c r="B29" s="38"/>
+      <c r="C29" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="93" t="s">
+      <c r="D29" s="36"/>
+      <c r="E29" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="93" t="s">
+      <c r="G29" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93" t="s">
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="51" t="s">
+      <c r="D30" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="93"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="109" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="109"/>
-      <c r="K30" s="51" t="s">
+      <c r="G30" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="122"/>
+      <c r="I30" s="122"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="L30" s="51" t="s">
+      <c r="L30" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="M30" s="51"/>
+      <c r="M30" s="36"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="51"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="93"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="109"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="109"/>
-      <c r="J31" s="109"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="122"/>
+      <c r="I31" s="122"/>
+      <c r="J31" s="122"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" s="17"/>
@@ -2591,13 +2540,13 @@
         <v/>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="109"/>
+      <c r="J32" s="109"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="76"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1">
       <c r="A33" s="17"/>
@@ -2615,13 +2564,13 @@
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="76"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
@@ -2642,13 +2591,13 @@
         <v/>
       </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
       <c r="A35" s="17"/>
@@ -2669,13 +2618,13 @@
         <v/>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1">
       <c r="A36" s="17"/>
@@ -2696,15 +2645,15 @@
         <v/>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
+      <c r="G36" s="109" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="109"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" s="17"/>
@@ -2725,13 +2674,13 @@
         <v/>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
       <c r="A38" s="17"/>
@@ -2752,13 +2701,13 @@
         <v/>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
       <c r="A39" s="17"/>
@@ -2779,15 +2728,15 @@
         <v/>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="38" t="s">
+      <c r="G39" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="40"/>
+      <c r="H39" s="144"/>
+      <c r="I39" s="144"/>
+      <c r="J39" s="144"/>
+      <c r="K39" s="144"/>
+      <c r="L39" s="144"/>
+      <c r="M39" s="145"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="17"/>
@@ -2808,15 +2757,15 @@
         <v/>
       </c>
       <c r="F40" s="7"/>
-      <c r="G40" s="110" t="s">
+      <c r="G40" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="112"/>
+      <c r="H40" s="124"/>
+      <c r="I40" s="124"/>
+      <c r="J40" s="124"/>
+      <c r="K40" s="124"/>
+      <c r="L40" s="124"/>
+      <c r="M40" s="125"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="15">
@@ -2834,203 +2783,203 @@
         <v>0</v>
       </c>
       <c r="F41" s="5"/>
-      <c r="G41" s="145" t="s">
+      <c r="G41" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="H41" s="145"/>
-      <c r="I41" s="145"/>
-      <c r="J41" s="145"/>
-      <c r="K41" s="102"/>
-      <c r="L41" s="102"/>
-      <c r="M41" s="102"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="115"/>
+      <c r="L41" s="115"/>
+      <c r="M41" s="115"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="155" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="156"/>
-      <c r="C42" s="156"/>
-      <c r="D42" s="156"/>
-      <c r="E42" s="156"/>
-      <c r="F42" s="156"/>
-      <c r="G42" s="156"/>
-      <c r="H42" s="157"/>
-      <c r="I42" s="103" t="s">
+      <c r="A42" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="J42" s="104"/>
-      <c r="K42" s="104"/>
-      <c r="L42" s="104"/>
-      <c r="M42" s="105"/>
+      <c r="J42" s="117"/>
+      <c r="K42" s="117"/>
+      <c r="L42" s="117"/>
+      <c r="M42" s="118"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="158"/>
-      <c r="B43" s="159"/>
-      <c r="C43" s="159"/>
-      <c r="D43" s="159"/>
-      <c r="E43" s="159"/>
-      <c r="F43" s="159"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="160"/>
-      <c r="I43" s="106" t="s">
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
+      <c r="M43" s="121"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A44" s="74"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="J44" s="113"/>
+      <c r="K44" s="113"/>
+      <c r="L44" s="113"/>
+      <c r="M44" s="114"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A45" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="107"/>
-      <c r="K43" s="107"/>
-      <c r="L43" s="107"/>
-      <c r="M43" s="108"/>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A44" s="161"/>
-      <c r="B44" s="142"/>
-      <c r="C44" s="142"/>
-      <c r="D44" s="142"/>
-      <c r="E44" s="142"/>
-      <c r="F44" s="142"/>
-      <c r="G44" s="142"/>
-      <c r="H44" s="162"/>
-      <c r="I44" s="99" t="s">
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="64"/>
+    </row>
+    <row r="46" spans="1:13" ht="30" customHeight="1">
+      <c r="A46" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="J44" s="100"/>
-      <c r="K44" s="100"/>
-      <c r="L44" s="100"/>
-      <c r="M44" s="101"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="52" t="s">
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="151"/>
-      <c r="C45" s="151"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="151"/>
-      <c r="F45" s="151"/>
-      <c r="G45" s="151"/>
-      <c r="H45" s="151"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="88"/>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1">
-      <c r="A46" s="96" t="s">
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="59"/>
+    </row>
+    <row r="47" spans="1:13" ht="19.5" customHeight="1">
+      <c r="A47" s="43"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="97"/>
-      <c r="C46" s="97"/>
-      <c r="D46" s="97"/>
-      <c r="E46" s="97"/>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="96" t="s">
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
+      <c r="L47" s="66"/>
+      <c r="M47" s="67"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A48" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="I46" s="97"/>
-      <c r="J46" s="97"/>
-      <c r="K46" s="97"/>
-      <c r="L46" s="97"/>
-      <c r="M46" s="98"/>
-    </row>
-    <row r="47" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A47" s="141"/>
-      <c r="B47" s="142"/>
-      <c r="C47" s="142"/>
-      <c r="D47" s="142"/>
-      <c r="E47" s="142"/>
-      <c r="F47" s="142"/>
-      <c r="G47" s="150"/>
-      <c r="H47" s="152" t="s">
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="I47" s="153"/>
-      <c r="J47" s="153"/>
-      <c r="K47" s="153"/>
-      <c r="L47" s="153"/>
-      <c r="M47" s="154"/>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="83" t="s">
+      <c r="F48" s="39"/>
+      <c r="G48" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="84"/>
-      <c r="C48" s="84"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="149" t="s">
+      <c r="H48" s="40"/>
+      <c r="I48" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="F48" s="138"/>
-      <c r="G48" s="138" t="s">
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="52"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A49" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H48" s="139"/>
-      <c r="I48" s="146" t="s">
-        <v>62</v>
-      </c>
-      <c r="J48" s="147"/>
-      <c r="K48" s="147"/>
-      <c r="L48" s="147"/>
-      <c r="M48" s="148"/>
-    </row>
-    <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="131" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="132"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="133"/>
-      <c r="E49" s="165" t="s">
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="42"/>
+      <c r="G49" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" s="46"/>
+      <c r="I49" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="32"/>
+    </row>
+    <row r="50" spans="1:13" ht="25.5" customHeight="1">
+      <c r="A50" s="30"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="42"/>
+      <c r="G50" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F49" s="140"/>
-      <c r="G49" s="164" t="s">
+      <c r="H50" s="46"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="32"/>
+    </row>
+    <row r="51" spans="1:13" ht="20.25" customHeight="1">
+      <c r="A51" s="33"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="H49" s="143"/>
-      <c r="I49" s="131" t="s">
-        <v>67</v>
-      </c>
-      <c r="J49" s="132"/>
-      <c r="K49" s="132"/>
-      <c r="L49" s="132"/>
-      <c r="M49" s="133"/>
-    </row>
-    <row r="50" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A50" s="131"/>
-      <c r="B50" s="132"/>
-      <c r="C50" s="132"/>
-      <c r="D50" s="133"/>
-      <c r="E50" s="165" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="140"/>
-      <c r="G50" s="164" t="s">
-        <v>96</v>
-      </c>
-      <c r="H50" s="143"/>
-      <c r="I50" s="131"/>
-      <c r="J50" s="132"/>
-      <c r="K50" s="132"/>
-      <c r="L50" s="132"/>
-      <c r="M50" s="133"/>
-    </row>
-    <row r="51" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A51" s="134"/>
-      <c r="B51" s="135"/>
-      <c r="C51" s="135"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="141"/>
-      <c r="F51" s="142"/>
-      <c r="G51" s="163" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="144"/>
-      <c r="I51" s="134"/>
-      <c r="J51" s="135"/>
-      <c r="K51" s="135"/>
-      <c r="L51" s="135"/>
-      <c r="M51" s="136"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="35"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="1"/>
@@ -3049,6 +2998,90 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="H5:M7"/>
+    <mergeCell ref="J22:M23"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="I44:M44"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="I42:M42"/>
+    <mergeCell ref="I43:M43"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="G30:J31"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M15"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="H16:M17"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="J19:M20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B24:E24"/>
     <mergeCell ref="I49:M51"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
@@ -3073,90 +3106,6 @@
     <mergeCell ref="A45:M45"/>
     <mergeCell ref="H47:M47"/>
     <mergeCell ref="A42:H44"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M15"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="H16:M17"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="J19:M20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="I44:M44"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="I42:M42"/>
-    <mergeCell ref="I43:M43"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="G30:J31"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="H5:M7"/>
-    <mergeCell ref="J22:M23"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A22:E23"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="G39:M39"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="H8:M8"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
@@ -3192,18 +3141,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="23">
         <v>1.45</v>
@@ -3214,7 +3163,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1">
       <c r="A3" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="23">
         <v>1</v>
@@ -3225,7 +3174,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="23">
         <v>1</v>
@@ -3236,7 +3185,7 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="23">
         <v>2.35</v>
@@ -3247,7 +3196,7 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="23">
         <v>4.5</v>
@@ -3258,7 +3207,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="24">
         <v>3</v>
@@ -3269,7 +3218,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="26">
         <v>4.5</v>
@@ -3280,7 +3229,7 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="24">
         <v>1.45</v>
@@ -3291,7 +3240,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="26">
         <v>1</v>
@@ -3302,7 +3251,7 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
@@ -3313,7 +3262,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="27">
         <v>1</v>
@@ -3324,7 +3273,7 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
@@ -3335,7 +3284,7 @@
     </row>
     <row r="14" spans="1:3" ht="16">
       <c r="A14" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
@@ -3346,7 +3295,7 @@
     </row>
     <row r="15" spans="1:3" ht="16">
       <c r="A15" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
@@ -3357,7 +3306,7 @@
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
@@ -3368,7 +3317,7 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
@@ -3387,15 +3336,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="27ba59cb-2538-41de-a2cb-c2b94feb3dc4" xsi:nil="true"/>
@@ -3404,6 +3344,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3630,20 +3579,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6401EDBB-EB38-4D67-8BC3-D6E86D979952}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93FEE14-9FD9-4703-9587-C4C577301079}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="27ba59cb-2538-41de-a2cb-c2b94feb3dc4"/>
     <ds:schemaRef ds:uri="e3877037-40d8-412e-928a-808df435ab6d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6401EDBB-EB38-4D67-8BC3-D6E86D979952}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
master bol - 2nd page logic
</commit_message>
<xml_diff>
--- a/template/template-target.xlsx
+++ b/template/template-target.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liajiang/Developers/BOL/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AB9CF-75E0-714E-B2C4-DB0CA49BB1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DDAE93-0FD3-7E49-9D4E-0CDCC78C466A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,6 +1020,317 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1038,12 +1349,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1089,42 +1394,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1156,284 +1434,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1895,7 +1895,7 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A33" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="I44" sqref="I44:M44"/>
     </sheetView>
   </sheetViews>
@@ -1911,446 +1911,446 @@
       <c r="A1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="142" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="161" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="161"/>
-      <c r="M1" s="162"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="126" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="127"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="129"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="130" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="131"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="133"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="76"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="130" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="139"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="89" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="91"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="79"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="91"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="94"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="82"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="163" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="164"/>
-      <c r="J8" s="164"/>
-      <c r="K8" s="164"/>
-      <c r="L8" s="164"/>
-      <c r="M8" s="165"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="146" t="s">
+      <c r="A9" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="147"/>
-      <c r="C9" s="147"/>
-      <c r="D9" s="147"/>
-      <c r="E9" s="147"/>
-      <c r="F9" s="147"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="77" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="79"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="82"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="113"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="149" t="s">
+      <c r="A11" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="150"/>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="151"/>
-      <c r="H11" s="83" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="85"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="116"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="86" t="s">
+      <c r="H12" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="88"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="119"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="89" t="s">
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="91"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="79"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="91"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="79"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="94"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="82"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="77"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="83" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="85"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="115"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="116"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="97"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="122"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="136"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="134" t="s">
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63" t="s">
+      <c r="I18" s="87"/>
+      <c r="J18" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63" t="s">
+      <c r="K18" s="87"/>
+      <c r="L18" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="64"/>
+      <c r="M18" s="88"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="77"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="107" t="s">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="108"/>
-      <c r="J19" s="103" t="s">
+      <c r="I19" s="130"/>
+      <c r="J19" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="103"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="104"/>
+      <c r="K19" s="125"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="126"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="80"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="156" t="s">
+      <c r="A20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="157"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="105"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="106"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="128"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="159"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G22" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="152" t="s">
+      <c r="H22" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="153"/>
-      <c r="J22" s="53" t="s">
+      <c r="I22" s="48"/>
+      <c r="J22" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="55"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="138"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="154" t="s">
+      <c r="A23" s="92"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="155"/>
-      <c r="J23" s="134"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="64"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="88"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="12" t="str">
         <f>IF(B24="", "", "PO#")</f>
         <v/>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="102"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="9" t="s">
@@ -2359,20 +2359,20 @@
       <c r="I24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="76"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="12" t="str">
         <f t="shared" ref="A25:A26" si="0">IF(B25="", "", "PO#")</f>
         <v/>
       </c>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="102"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="124"/>
       <c r="F25" s="17"/>
       <c r="G25" s="19"/>
       <c r="H25" s="6" t="s">
@@ -2381,20 +2381,20 @@
       <c r="I25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B26" s="101"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102"/>
+      <c r="B26" s="123"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="124"/>
       <c r="F26" s="17"/>
       <c r="G26" s="19"/>
       <c r="H26" s="6" t="s">
@@ -2403,19 +2403,19 @@
       <c r="I26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="13">
         <f>F24+F25</f>
         <v>0</v>
@@ -2424,104 +2424,104 @@
         <f>G24+G25</f>
         <v>0</v>
       </c>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
+      <c r="M27" s="94"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="111" t="s">
+      <c r="A28" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="111"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="111"/>
-      <c r="M28" s="111"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="95"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="36" t="s">
+      <c r="B29" s="137"/>
+      <c r="C29" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37" t="s">
+      <c r="D29" s="51"/>
+      <c r="E29" s="93" t="s">
         <v>32</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37" t="s">
+      <c r="H29" s="93"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="37"/>
+      <c r="E30" s="93"/>
       <c r="F30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="122" t="s">
+      <c r="G30" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="122"/>
-      <c r="I30" s="122"/>
-      <c r="J30" s="122"/>
-      <c r="K30" s="36" t="s">
+      <c r="H30" s="109"/>
+      <c r="I30" s="109"/>
+      <c r="J30" s="109"/>
+      <c r="K30" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="L30" s="36" t="s">
+      <c r="L30" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="M30" s="36"/>
+      <c r="M30" s="51"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="93"/>
       <c r="F31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="122"/>
-      <c r="H31" s="122"/>
-      <c r="I31" s="122"/>
-      <c r="J31" s="122"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-    </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+    </row>
+    <row r="32" spans="1:13" ht="27" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="4" t="str">
         <f>IF(A32="","","Units")</f>
@@ -2540,15 +2540,15 @@
         <v/>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="109"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-    </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1">
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="4" t="str">
         <f t="shared" ref="B33:B40" si="1">IF(A33="","","Units")</f>
@@ -2564,15 +2564,15 @@
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="109"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" ht="26" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="4" t="str">
         <f t="shared" ref="B34:B35" si="3">IF(A34="","","Units")</f>
@@ -2591,15 +2591,15 @@
         <v/>
       </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="4" t="str">
         <f t="shared" si="3"/>
@@ -2618,15 +2618,15 @@
         <v/>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="109"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" ht="27" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2645,17 +2645,17 @@
         <v/>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="109" t="s">
+      <c r="G36" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="109"/>
-      <c r="I36" s="109"/>
-      <c r="J36" s="109"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" ht="26" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2674,15 +2674,15 @@
         <v/>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="109"/>
-      <c r="I37" s="109"/>
-      <c r="J37" s="109"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" ht="27" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2701,15 +2701,15 @@
         <v/>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="109"/>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="109"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" ht="23" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2728,15 +2728,15 @@
         <v/>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="143" t="s">
+      <c r="G39" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H39" s="144"/>
-      <c r="I39" s="144"/>
-      <c r="J39" s="144"/>
-      <c r="K39" s="144"/>
-      <c r="L39" s="144"/>
-      <c r="M39" s="145"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="40"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="17"/>
@@ -2757,15 +2757,15 @@
         <v/>
       </c>
       <c r="F40" s="7"/>
-      <c r="G40" s="123" t="s">
+      <c r="G40" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="H40" s="124"/>
-      <c r="I40" s="124"/>
-      <c r="J40" s="124"/>
-      <c r="K40" s="124"/>
-      <c r="L40" s="124"/>
-      <c r="M40" s="125"/>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111"/>
+      <c r="J40" s="111"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="112"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="15">
@@ -2783,203 +2783,203 @@
         <v>0</v>
       </c>
       <c r="F41" s="5"/>
-      <c r="G41" s="49" t="s">
+      <c r="G41" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="H41" s="49"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="115"/>
-      <c r="L41" s="115"/>
-      <c r="M41" s="115"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="148"/>
+      <c r="J41" s="148"/>
+      <c r="K41" s="102"/>
+      <c r="L41" s="102"/>
+      <c r="M41" s="102"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="68" t="s">
+      <c r="A42" s="158" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="116" t="s">
+      <c r="B42" s="159"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="159"/>
+      <c r="H42" s="160"/>
+      <c r="I42" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="J42" s="117"/>
-      <c r="K42" s="117"/>
-      <c r="L42" s="117"/>
-      <c r="M42" s="118"/>
+      <c r="J42" s="104"/>
+      <c r="K42" s="104"/>
+      <c r="L42" s="104"/>
+      <c r="M42" s="105"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="73"/>
-      <c r="I43" s="119" t="s">
+      <c r="A43" s="161"/>
+      <c r="B43" s="162"/>
+      <c r="C43" s="162"/>
+      <c r="D43" s="162"/>
+      <c r="E43" s="162"/>
+      <c r="F43" s="162"/>
+      <c r="G43" s="162"/>
+      <c r="H43" s="163"/>
+      <c r="I43" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="J43" s="120"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
-      <c r="M43" s="121"/>
+      <c r="J43" s="107"/>
+      <c r="K43" s="107"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="108"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A44" s="74"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="112" t="s">
+      <c r="A44" s="164"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="143"/>
+      <c r="D44" s="143"/>
+      <c r="E44" s="143"/>
+      <c r="F44" s="143"/>
+      <c r="G44" s="143"/>
+      <c r="H44" s="165"/>
+      <c r="I44" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="J44" s="113"/>
-      <c r="K44" s="113"/>
-      <c r="L44" s="113"/>
-      <c r="M44" s="114"/>
+      <c r="J44" s="100"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="100"/>
+      <c r="M44" s="101"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="61" t="s">
+      <c r="A45" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="64"/>
+      <c r="B45" s="154"/>
+      <c r="C45" s="154"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="154"/>
+      <c r="H45" s="154"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="88"/>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="57" t="s">
+      <c r="B46" s="97"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="97"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="59"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="97"/>
+      <c r="K46" s="97"/>
+      <c r="L46" s="97"/>
+      <c r="M46" s="98"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A47" s="43"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="65" t="s">
+      <c r="A47" s="142"/>
+      <c r="B47" s="143"/>
+      <c r="C47" s="143"/>
+      <c r="D47" s="143"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="143"/>
+      <c r="G47" s="153"/>
+      <c r="H47" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="66"/>
-      <c r="L47" s="66"/>
-      <c r="M47" s="67"/>
+      <c r="I47" s="156"/>
+      <c r="J47" s="156"/>
+      <c r="K47" s="156"/>
+      <c r="L47" s="156"/>
+      <c r="M47" s="157"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="53" t="s">
+      <c r="A48" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="54"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56" t="s">
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39" t="s">
+      <c r="F48" s="138"/>
+      <c r="G48" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="H48" s="40"/>
-      <c r="I48" s="50" t="s">
+      <c r="H48" s="139"/>
+      <c r="I48" s="149" t="s">
         <v>60</v>
       </c>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="52"/>
+      <c r="J48" s="150"/>
+      <c r="K48" s="150"/>
+      <c r="L48" s="150"/>
+      <c r="M48" s="151"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="41" t="s">
+      <c r="B49" s="132"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="133"/>
+      <c r="E49" s="140" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="42"/>
-      <c r="G49" s="45" t="s">
+      <c r="F49" s="141"/>
+      <c r="G49" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="H49" s="46"/>
-      <c r="I49" s="30" t="s">
+      <c r="H49" s="145"/>
+      <c r="I49" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="J49" s="31"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="32"/>
+      <c r="J49" s="132"/>
+      <c r="K49" s="132"/>
+      <c r="L49" s="132"/>
+      <c r="M49" s="133"/>
     </row>
     <row r="50" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="41" t="s">
+      <c r="A50" s="131"/>
+      <c r="B50" s="132"/>
+      <c r="C50" s="132"/>
+      <c r="D50" s="133"/>
+      <c r="E50" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="42"/>
-      <c r="G50" s="45" t="s">
+      <c r="F50" s="141"/>
+      <c r="G50" s="144" t="s">
         <v>94</v>
       </c>
-      <c r="H50" s="46"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="32"/>
+      <c r="H50" s="145"/>
+      <c r="I50" s="131"/>
+      <c r="J50" s="132"/>
+      <c r="K50" s="132"/>
+      <c r="L50" s="132"/>
+      <c r="M50" s="133"/>
     </row>
     <row r="51" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A51" s="33"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="47" t="s">
+      <c r="A51" s="134"/>
+      <c r="B51" s="135"/>
+      <c r="C51" s="135"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="143"/>
+      <c r="G51" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="H51" s="48"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="35"/>
+      <c r="H51" s="147"/>
+      <c r="I51" s="134"/>
+      <c r="J51" s="135"/>
+      <c r="K51" s="135"/>
+      <c r="L51" s="135"/>
+      <c r="M51" s="136"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="1"/>
@@ -2998,6 +2998,90 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="I49:M51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D51"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="A46:G47"/>
+    <mergeCell ref="A45:M45"/>
+    <mergeCell ref="H47:M47"/>
+    <mergeCell ref="A42:H44"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M15"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="H16:M17"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="J19:M20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="I44:M44"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="I42:M42"/>
+    <mergeCell ref="I43:M43"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="G30:J31"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="H5:M7"/>
+    <mergeCell ref="J22:M23"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A22:E23"/>
     <mergeCell ref="G37:J37"/>
     <mergeCell ref="L37:M37"/>
     <mergeCell ref="G38:J38"/>
@@ -3022,90 +3106,6 @@
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="H5:M7"/>
-    <mergeCell ref="J22:M23"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A22:E23"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="I44:M44"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="I42:M42"/>
-    <mergeCell ref="I43:M43"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="G30:J31"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M15"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="H16:M17"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="J19:M20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="I49:M51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="I48:M48"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D51"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="A46:G47"/>
-    <mergeCell ref="A45:M45"/>
-    <mergeCell ref="H47:M47"/>
-    <mergeCell ref="A42:H44"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
@@ -3336,26 +3336,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="27ba59cb-2538-41de-a2cb-c2b94feb3dc4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3877037-40d8-412e-928a-808df435ab6d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010021B2BA11543C6E46B0BDC5084A8D08CB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4560cc6e5f86f0938f3e5e1e4c9b8f7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3877037-40d8-412e-928a-808df435ab6d" xmlns:ns3="27ba59cb-2538-41de-a2cb-c2b94feb3dc4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3181f8747d74a5910393c39a7dfff70a" ns2:_="" ns3:_="">
     <xsd:import namespace="e3877037-40d8-412e-928a-808df435ab6d"/>
@@ -3578,26 +3558,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93FEE14-9FD9-4703-9587-C4C577301079}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27ba59cb-2538-41de-a2cb-c2b94feb3dc4"/>
-    <ds:schemaRef ds:uri="e3877037-40d8-412e-928a-808df435ab6d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6401EDBB-EB38-4D67-8BC3-D6E86D979952}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="27ba59cb-2538-41de-a2cb-c2b94feb3dc4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3877037-40d8-412e-928a-808df435ab6d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5827C6D-1863-4DB6-987C-8BB728710A3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3614,4 +3595,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6401EDBB-EB38-4D67-8BC3-D6E86D979952}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93FEE14-9FD9-4703-9587-C4C577301079}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27ba59cb-2538-41de-a2cb-c2b94feb3dc4"/>
+    <ds:schemaRef ds:uri="e3877037-40d8-412e-928a-808df435ab6d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>